<commit_message>
new plot and make slide
</commit_message>
<xml_diff>
--- a/parameters_model.xlsx
+++ b/parameters_model.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>vector_size</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>True, False ?</t>
+  </si>
+  <si>
+    <t>min_n</t>
+  </si>
+  <si>
+    <t>max_n</t>
+  </si>
+  <si>
+    <t>bucket</t>
   </si>
 </sst>
 </file>
@@ -403,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +430,7 @@
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,8 +470,56 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -470,7 +527,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -479,7 +536,10 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
       </c>
       <c r="H2">
         <v>1</v>

</xml_diff>

<commit_message>
plot histogram of freq skill and len jd
</commit_message>
<xml_diff>
--- a/parameters_model.xlsx
+++ b/parameters_model.xlsx
@@ -415,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF6"/>
+  <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AC8" sqref="AC8"/>
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +959,219 @@
         <v>3000000</v>
       </c>
       <c r="AF6">
-        <v>0.22350868859597001</v>
+        <v>0.22623995566638899</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>100</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>12</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>100</v>
+      </c>
+      <c r="Y7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>0.1</v>
+      </c>
+      <c r="AA7">
+        <v>6</v>
+      </c>
+      <c r="AB7">
+        <v>200</v>
+      </c>
+      <c r="AC7">
+        <v>5</v>
+      </c>
+      <c r="AD7">
+        <v>7</v>
+      </c>
+      <c r="AE7">
+        <v>3000000</v>
+      </c>
+      <c r="AF7">
+        <v>0.22268403066407999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>100</v>
+      </c>
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="R8">
+        <v>12</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>100</v>
+      </c>
+      <c r="Y8" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0.1</v>
+      </c>
+      <c r="AA8">
+        <v>6</v>
+      </c>
+      <c r="AB8">
+        <v>200</v>
+      </c>
+      <c r="AC8">
+        <v>5</v>
+      </c>
+      <c r="AD8">
+        <v>8</v>
+      </c>
+      <c r="AE8">
+        <v>3000000</v>
+      </c>
+      <c r="AF8">
+        <v>0.22268403066407999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>100</v>
+      </c>
+      <c r="Q9">
+        <v>2</v>
+      </c>
+      <c r="R9">
+        <v>12</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>100</v>
+      </c>
+      <c r="Y9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <v>0.1</v>
+      </c>
+      <c r="AA9">
+        <v>6</v>
+      </c>
+      <c r="AB9">
+        <v>200</v>
+      </c>
+      <c r="AC9">
+        <v>5</v>
+      </c>
+      <c r="AD9">
+        <v>7</v>
+      </c>
+      <c r="AE9">
+        <v>3000000</v>
+      </c>
+      <c r="AF9">
+        <v>0.22268403066407999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>100</v>
+      </c>
+      <c r="Q10">
+        <v>2</v>
+      </c>
+      <c r="R10">
+        <v>12</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <v>100</v>
+      </c>
+      <c r="Y10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>0.1</v>
+      </c>
+      <c r="AA10">
+        <v>6</v>
+      </c>
+      <c r="AB10">
+        <v>200</v>
+      </c>
+      <c r="AC10">
+        <v>5</v>
+      </c>
+      <c r="AD10">
+        <v>7</v>
+      </c>
+      <c r="AE10">
+        <v>3000000</v>
+      </c>
+      <c r="AF10">
+        <v>0.22268403066407999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done overview of data and data processing issue #2
</commit_message>
<xml_diff>
--- a/parameters_model.xlsx
+++ b/parameters_model.xlsx
@@ -415,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF10"/>
+  <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC30" sqref="AC30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,6 +572,9 @@
       <c r="N2">
         <v>0.21736880657495899</v>
       </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
       <c r="P2">
         <v>100</v>
       </c>
@@ -667,6 +670,9 @@
       <c r="N3">
         <v>0.21260424576800799</v>
       </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
       <c r="P3">
         <v>100</v>
       </c>
@@ -762,6 +768,9 @@
       <c r="N4">
         <v>0.232529383698347</v>
       </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
       <c r="P4">
         <v>100</v>
       </c>
@@ -857,6 +866,9 @@
       <c r="N5">
         <v>0.224955815250626</v>
       </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
       <c r="P5">
         <v>100</v>
       </c>
@@ -910,6 +922,9 @@
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>5</v>
+      </c>
       <c r="P6">
         <v>100</v>
       </c>
@@ -963,6 +978,9 @@
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>6</v>
+      </c>
       <c r="P7">
         <v>100</v>
       </c>
@@ -1016,6 +1034,9 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>7</v>
+      </c>
       <c r="P8">
         <v>100</v>
       </c>
@@ -1069,6 +1090,9 @@
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>8</v>
+      </c>
       <c r="P9">
         <v>100</v>
       </c>
@@ -1112,7 +1136,7 @@
         <v>5</v>
       </c>
       <c r="AD9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE9">
         <v>3000000</v>
@@ -1122,11 +1146,14 @@
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>9</v>
+      </c>
       <c r="P10">
         <v>100</v>
       </c>
       <c r="Q10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R10">
         <v>12</v>
@@ -1150,7 +1177,7 @@
         <v>100</v>
       </c>
       <c r="Y10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z10">
         <v>0.1</v>
@@ -1162,7 +1189,7 @@
         <v>200</v>
       </c>
       <c r="AC10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AD10">
         <v>7</v>
@@ -1171,7 +1198,399 @@
         <v>3000000</v>
       </c>
       <c r="AF10">
-        <v>0.22268403066407999</v>
+        <v>0.23479000910422301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>10</v>
+      </c>
+      <c r="P11">
+        <v>100</v>
+      </c>
+      <c r="Q11">
+        <v>3</v>
+      </c>
+      <c r="R11">
+        <v>12</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>100</v>
+      </c>
+      <c r="Y11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>0.1</v>
+      </c>
+      <c r="AA11">
+        <v>6</v>
+      </c>
+      <c r="AB11">
+        <v>200</v>
+      </c>
+      <c r="AC11">
+        <v>3</v>
+      </c>
+      <c r="AD11">
+        <v>7</v>
+      </c>
+      <c r="AE11">
+        <v>3000000</v>
+      </c>
+      <c r="AF11">
+        <v>0.229657338136141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <v>11</v>
+      </c>
+      <c r="P12">
+        <v>100</v>
+      </c>
+      <c r="Q12">
+        <v>3</v>
+      </c>
+      <c r="R12">
+        <v>12</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>100</v>
+      </c>
+      <c r="Y12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0.1</v>
+      </c>
+      <c r="AA12">
+        <v>6</v>
+      </c>
+      <c r="AB12">
+        <v>200</v>
+      </c>
+      <c r="AC12">
+        <v>3</v>
+      </c>
+      <c r="AD12">
+        <v>8</v>
+      </c>
+      <c r="AE12">
+        <v>3000000</v>
+      </c>
+      <c r="AF12">
+        <v>0.23554869440156201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>12</v>
+      </c>
+      <c r="P13">
+        <v>100</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13">
+        <v>12</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <v>100</v>
+      </c>
+      <c r="Y13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <v>0.1</v>
+      </c>
+      <c r="AA13">
+        <v>6</v>
+      </c>
+      <c r="AB13">
+        <v>200</v>
+      </c>
+      <c r="AC13">
+        <v>3</v>
+      </c>
+      <c r="AD13">
+        <v>8</v>
+      </c>
+      <c r="AE13">
+        <v>3000000</v>
+      </c>
+      <c r="AF13">
+        <v>0.23066012218131901</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <v>13</v>
+      </c>
+      <c r="P14">
+        <v>100</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+      <c r="R14">
+        <v>12</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>100</v>
+      </c>
+      <c r="Y14" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0.1</v>
+      </c>
+      <c r="AA14">
+        <v>6</v>
+      </c>
+      <c r="AB14">
+        <v>200</v>
+      </c>
+      <c r="AC14">
+        <v>5</v>
+      </c>
+      <c r="AD14">
+        <v>7</v>
+      </c>
+      <c r="AE14">
+        <v>3000000</v>
+      </c>
+      <c r="AF14">
+        <v>0.23907163308659499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>14</v>
+      </c>
+      <c r="P15">
+        <v>100</v>
+      </c>
+      <c r="Q15">
+        <v>3</v>
+      </c>
+      <c r="R15">
+        <v>12</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <v>100</v>
+      </c>
+      <c r="Y15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>0.1</v>
+      </c>
+      <c r="AA15">
+        <v>6</v>
+      </c>
+      <c r="AB15">
+        <v>200</v>
+      </c>
+      <c r="AC15">
+        <v>5</v>
+      </c>
+      <c r="AD15">
+        <v>7</v>
+      </c>
+      <c r="AE15">
+        <v>3000000</v>
+      </c>
+      <c r="AF15">
+        <v>0.23371465516103901</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <v>15</v>
+      </c>
+      <c r="P16">
+        <v>100</v>
+      </c>
+      <c r="Q16">
+        <v>3</v>
+      </c>
+      <c r="R16">
+        <v>12</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>100</v>
+      </c>
+      <c r="Y16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0.1</v>
+      </c>
+      <c r="AA16">
+        <v>6</v>
+      </c>
+      <c r="AB16">
+        <v>200</v>
+      </c>
+      <c r="AC16">
+        <v>5</v>
+      </c>
+      <c r="AD16">
+        <v>8</v>
+      </c>
+      <c r="AE16">
+        <v>3000000</v>
+      </c>
+      <c r="AF16">
+        <v>0.239124411194236</v>
+      </c>
+    </row>
+    <row r="17" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>16</v>
+      </c>
+      <c r="P17">
+        <v>100</v>
+      </c>
+      <c r="Q17">
+        <v>3</v>
+      </c>
+      <c r="R17">
+        <v>12</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17">
+        <v>100</v>
+      </c>
+      <c r="Y17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>0.1</v>
+      </c>
+      <c r="AA17">
+        <v>6</v>
+      </c>
+      <c r="AB17">
+        <v>200</v>
+      </c>
+      <c r="AC17">
+        <v>5</v>
+      </c>
+      <c r="AD17">
+        <v>8</v>
+      </c>
+      <c r="AE17">
+        <v>3000000</v>
+      </c>
+      <c r="AF17">
+        <v>0.23333201388064201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update slide valid data issue #2
</commit_message>
<xml_diff>
--- a/parameters_model.xlsx
+++ b/parameters_model.xlsx
@@ -415,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF17"/>
+  <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC30" sqref="AC30"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AB34" sqref="AB34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,8 +1593,635 @@
         <v>0.23333201388064201</v>
       </c>
     </row>
+    <row r="18" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <v>17</v>
+      </c>
+      <c r="P18">
+        <v>100</v>
+      </c>
+      <c r="Q18">
+        <v>3</v>
+      </c>
+      <c r="R18">
+        <v>12</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>2</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18">
+        <v>100</v>
+      </c>
+      <c r="Y18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0.1</v>
+      </c>
+      <c r="AA18">
+        <v>6</v>
+      </c>
+      <c r="AB18">
+        <v>200</v>
+      </c>
+      <c r="AC18">
+        <v>3</v>
+      </c>
+      <c r="AD18">
+        <v>7</v>
+      </c>
+      <c r="AE18">
+        <v>3000000</v>
+      </c>
+      <c r="AF18">
+        <v>0.16502394806634199</v>
+      </c>
+    </row>
+    <row r="19" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>18</v>
+      </c>
+      <c r="P19">
+        <v>100</v>
+      </c>
+      <c r="Q19">
+        <v>3</v>
+      </c>
+      <c r="R19">
+        <v>12</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19">
+        <v>100</v>
+      </c>
+      <c r="Z19">
+        <v>0.1</v>
+      </c>
+      <c r="AA19">
+        <v>6</v>
+      </c>
+      <c r="AB19">
+        <v>200</v>
+      </c>
+      <c r="AE19">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="20" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <v>19</v>
+      </c>
+      <c r="P20">
+        <v>100</v>
+      </c>
+      <c r="Q20">
+        <v>3</v>
+      </c>
+      <c r="R20">
+        <v>12</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <v>100</v>
+      </c>
+      <c r="Z20">
+        <v>0.1</v>
+      </c>
+      <c r="AA20">
+        <v>6</v>
+      </c>
+      <c r="AB20">
+        <v>200</v>
+      </c>
+      <c r="AE20">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="21" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <v>20</v>
+      </c>
+      <c r="P21">
+        <v>100</v>
+      </c>
+      <c r="Q21">
+        <v>3</v>
+      </c>
+      <c r="R21">
+        <v>12</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21">
+        <v>100</v>
+      </c>
+      <c r="Z21">
+        <v>0.1</v>
+      </c>
+      <c r="AA21">
+        <v>6</v>
+      </c>
+      <c r="AB21">
+        <v>200</v>
+      </c>
+      <c r="AE21">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="22" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <v>21</v>
+      </c>
+      <c r="P22">
+        <v>100</v>
+      </c>
+      <c r="Q22">
+        <v>3</v>
+      </c>
+      <c r="R22">
+        <v>12</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22">
+        <v>100</v>
+      </c>
+      <c r="Z22">
+        <v>0.1</v>
+      </c>
+      <c r="AA22">
+        <v>6</v>
+      </c>
+      <c r="AB22">
+        <v>200</v>
+      </c>
+      <c r="AE22">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="23" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <v>22</v>
+      </c>
+      <c r="P23">
+        <v>100</v>
+      </c>
+      <c r="Q23">
+        <v>3</v>
+      </c>
+      <c r="R23">
+        <v>12</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23">
+        <v>100</v>
+      </c>
+      <c r="Z23">
+        <v>0.1</v>
+      </c>
+      <c r="AA23">
+        <v>6</v>
+      </c>
+      <c r="AB23">
+        <v>200</v>
+      </c>
+      <c r="AE23">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="24" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>23</v>
+      </c>
+      <c r="P24">
+        <v>100</v>
+      </c>
+      <c r="Q24">
+        <v>3</v>
+      </c>
+      <c r="R24">
+        <v>12</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24">
+        <v>100</v>
+      </c>
+      <c r="Z24">
+        <v>0.1</v>
+      </c>
+      <c r="AA24">
+        <v>6</v>
+      </c>
+      <c r="AB24">
+        <v>200</v>
+      </c>
+      <c r="AE24">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="25" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <v>24</v>
+      </c>
+      <c r="P25">
+        <v>100</v>
+      </c>
+      <c r="Q25">
+        <v>3</v>
+      </c>
+      <c r="R25">
+        <v>12</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="X25">
+        <v>100</v>
+      </c>
+      <c r="Z25">
+        <v>0.1</v>
+      </c>
+      <c r="AA25">
+        <v>6</v>
+      </c>
+      <c r="AB25">
+        <v>200</v>
+      </c>
+      <c r="AE25">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="26" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <v>25</v>
+      </c>
+      <c r="P26">
+        <v>100</v>
+      </c>
+      <c r="Q26">
+        <v>3</v>
+      </c>
+      <c r="R26">
+        <v>12</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
+      </c>
+      <c r="X26">
+        <v>100</v>
+      </c>
+      <c r="Z26">
+        <v>0.1</v>
+      </c>
+      <c r="AA26">
+        <v>6</v>
+      </c>
+      <c r="AB26">
+        <v>200</v>
+      </c>
+      <c r="AE26">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="27" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <v>26</v>
+      </c>
+      <c r="P27">
+        <v>100</v>
+      </c>
+      <c r="Q27">
+        <v>3</v>
+      </c>
+      <c r="R27">
+        <v>12</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="W27">
+        <v>1</v>
+      </c>
+      <c r="X27">
+        <v>100</v>
+      </c>
+      <c r="Z27">
+        <v>0.1</v>
+      </c>
+      <c r="AA27">
+        <v>6</v>
+      </c>
+      <c r="AB27">
+        <v>200</v>
+      </c>
+      <c r="AE27">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="28" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O28">
+        <v>27</v>
+      </c>
+      <c r="P28">
+        <v>100</v>
+      </c>
+      <c r="Q28">
+        <v>3</v>
+      </c>
+      <c r="R28">
+        <v>12</v>
+      </c>
+      <c r="S28">
+        <v>1</v>
+      </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
+      <c r="W28">
+        <v>1</v>
+      </c>
+      <c r="X28">
+        <v>100</v>
+      </c>
+      <c r="Z28">
+        <v>0.1</v>
+      </c>
+      <c r="AA28">
+        <v>6</v>
+      </c>
+      <c r="AB28">
+        <v>200</v>
+      </c>
+      <c r="AE28">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="29" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <v>28</v>
+      </c>
+      <c r="P29">
+        <v>100</v>
+      </c>
+      <c r="Q29">
+        <v>3</v>
+      </c>
+      <c r="R29">
+        <v>12</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="W29">
+        <v>1</v>
+      </c>
+      <c r="X29">
+        <v>100</v>
+      </c>
+      <c r="Z29">
+        <v>0.1</v>
+      </c>
+      <c r="AA29">
+        <v>6</v>
+      </c>
+      <c r="AB29">
+        <v>200</v>
+      </c>
+      <c r="AE29">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="30" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <v>29</v>
+      </c>
+      <c r="P30">
+        <v>100</v>
+      </c>
+      <c r="Q30">
+        <v>3</v>
+      </c>
+      <c r="R30">
+        <v>12</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <v>1</v>
+      </c>
+      <c r="W30">
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <v>100</v>
+      </c>
+      <c r="Z30">
+        <v>0.1</v>
+      </c>
+      <c r="AA30">
+        <v>6</v>
+      </c>
+      <c r="AB30">
+        <v>200</v>
+      </c>
+      <c r="AE30">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="31" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <v>30</v>
+      </c>
+      <c r="P31">
+        <v>100</v>
+      </c>
+      <c r="Q31">
+        <v>3</v>
+      </c>
+      <c r="R31">
+        <v>12</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+      <c r="T31">
+        <v>1</v>
+      </c>
+      <c r="W31">
+        <v>1</v>
+      </c>
+      <c r="X31">
+        <v>100</v>
+      </c>
+      <c r="Z31">
+        <v>0.1</v>
+      </c>
+      <c r="AA31">
+        <v>6</v>
+      </c>
+      <c r="AB31">
+        <v>200</v>
+      </c>
+      <c r="AE31">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="32" spans="15:32" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <v>31</v>
+      </c>
+      <c r="P32">
+        <v>100</v>
+      </c>
+      <c r="Q32">
+        <v>3</v>
+      </c>
+      <c r="R32">
+        <v>12</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <v>1</v>
+      </c>
+      <c r="X32">
+        <v>100</v>
+      </c>
+      <c r="Z32">
+        <v>0.1</v>
+      </c>
+      <c r="AA32">
+        <v>6</v>
+      </c>
+      <c r="AB32">
+        <v>200</v>
+      </c>
+      <c r="AE32">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="33" spans="15:31" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <v>32</v>
+      </c>
+      <c r="P33">
+        <v>100</v>
+      </c>
+      <c r="Q33">
+        <v>3</v>
+      </c>
+      <c r="R33">
+        <v>12</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="T33">
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <v>1</v>
+      </c>
+      <c r="X33">
+        <v>100</v>
+      </c>
+      <c r="Z33">
+        <v>0.1</v>
+      </c>
+      <c r="AA33">
+        <v>6</v>
+      </c>
+      <c r="AB33">
+        <v>200</v>
+      </c>
+      <c r="AE33">
+        <v>3000000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>